<commit_message>
Added average stats after subsampling
</commit_message>
<xml_diff>
--- a/Metrics Table.xlsx
+++ b/Metrics Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abheesht\Documents\Academics\SOP\Snehanshu\Support Vector Economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D13E46B-4BA3-4865-B368-35FEF8571BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD4232A-A9CD-46C3-BD49-7F07BAFA6AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E7CF4481-218E-4EC8-9CC8-6BD847CFA7F6}"/>
   </bookViews>
@@ -42,12 +42,6 @@
     <t>Polynomial</t>
   </si>
   <si>
-    <t>Training Metrics</t>
-  </si>
-  <si>
-    <t>Test Metrics</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>Degree 2</t>
+  </si>
+  <si>
+    <t>Average Training Metrics</t>
+  </si>
+  <si>
+    <t>Average Test Metrics</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,16 +505,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -531,56 +531,50 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.56999999999999995</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>0.63</v>
+        <v>0.73</v>
       </c>
       <c r="C4" s="1">
-        <v>0.62</v>
+        <v>0.74</v>
       </c>
       <c r="D4" s="1">
-        <v>0.97</v>
+        <v>0.84</v>
       </c>
       <c r="E4" s="1">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="F4" s="1">
         <v>0.6</v>
@@ -589,10 +583,10 @@
         <v>0.6</v>
       </c>
       <c r="H4" s="1">
-        <v>0.97</v>
+        <v>0.68</v>
       </c>
       <c r="I4" s="1">
-        <v>0.74</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -602,45 +596,45 @@
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="C6" s="1">
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="D6" s="1">
-        <v>0.98</v>
+        <v>0.85</v>
       </c>
       <c r="E6" s="1">
-        <v>0.75</v>
+        <v>0.72</v>
       </c>
       <c r="F6" s="1">
-        <v>0.59</v>
+        <v>0.53</v>
       </c>
       <c r="G6" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.53</v>
       </c>
       <c r="H6" s="1">
-        <v>0.99</v>
+        <v>0.62</v>
       </c>
       <c r="I6" s="1">
-        <v>0.73</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>0.62</v>
+        <v>0.67</v>
       </c>
       <c r="C7" s="1">
-        <v>0.61</v>
+        <v>0.66</v>
       </c>
       <c r="D7" s="1">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="E7" s="1">
         <v>0.76</v>
@@ -649,236 +643,284 @@
         <v>0.59</v>
       </c>
       <c r="G7" s="1">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H7" s="1">
-        <v>0.98</v>
+        <v>0.85</v>
       </c>
       <c r="I7" s="1">
-        <v>0.73</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
-        <v>0.62</v>
+        <v>0.66</v>
       </c>
       <c r="C8" s="1">
-        <v>0.61</v>
+        <v>0.7</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0.82</v>
       </c>
       <c r="E8" s="1">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
       <c r="F8" s="1">
-        <v>0.6</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G8" s="1">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H8" s="1">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="I8" s="1">
-        <v>0.74</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="C9" s="1">
-        <v>0.62</v>
+        <v>0.72</v>
       </c>
       <c r="D9" s="1">
-        <v>0.99</v>
+        <v>0.83</v>
       </c>
       <c r="E9" s="1">
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="F9" s="1">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="G9" s="1">
-        <v>0.59</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H9" s="1">
-        <v>0.98</v>
+        <v>0.73</v>
       </c>
       <c r="I9" s="1">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="C10" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.62</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.59</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.99</v>
-      </c>
       <c r="I10" s="1">
-        <v>0.74</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>0.64</v>
+        <v>0.7</v>
       </c>
       <c r="C11" s="1">
-        <v>0.62</v>
+        <v>0.74</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="E11" s="1">
-        <v>0.77</v>
+        <v>0.74</v>
       </c>
       <c r="F11" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="I11" s="1">
         <v>0.6</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.59</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.74</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="C12" s="1">
-        <v>0.63</v>
+        <v>0.74</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="E12" s="1">
-        <v>0.77</v>
+        <v>0.74</v>
       </c>
       <c r="F12" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.6</v>
       </c>
-      <c r="G12" s="1">
-        <v>0.59</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.98</v>
-      </c>
       <c r="I12" s="1">
-        <v>0.74</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="C13" s="1">
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="E13" s="1">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="F13" s="1">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G13" s="1">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
       <c r="H13" s="1">
-        <v>0.98</v>
+        <v>0.69</v>
       </c>
       <c r="I13" s="1">
-        <v>0.74</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="C14" s="1">
-        <v>0.63</v>
+        <v>0.77</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E14" s="1">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="F14" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.6</v>
       </c>
-      <c r="G14" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.98</v>
-      </c>
       <c r="I14" s="1">
-        <v>0.74</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.54</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
         <v>0.59</v>
@@ -893,21 +935,21 @@
         <v>0.74</v>
       </c>
       <c r="F18" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G18" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
       </c>
       <c r="I18" s="1">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>0.59</v>
@@ -922,21 +964,21 @@
         <v>0.74</v>
       </c>
       <c r="F19" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G19" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
       </c>
       <c r="I19" s="1">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>0.59</v>
@@ -951,21 +993,21 @@
         <v>0.74</v>
       </c>
       <c r="F20" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G20" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
       </c>
       <c r="I20" s="1">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>0.59</v>
@@ -980,21 +1022,21 @@
         <v>0.74</v>
       </c>
       <c r="F21" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G21" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
       </c>
       <c r="I21" s="1">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>0.59</v>
@@ -1009,21 +1051,21 @@
         <v>0.74</v>
       </c>
       <c r="F22" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G22" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
       </c>
       <c r="I22" s="1">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1">
         <v>0.59</v>
@@ -1038,16 +1080,16 @@
         <v>0.74</v>
       </c>
       <c r="F23" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G23" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
       <c r="I23" s="1">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>